<commit_message>
Updated property code descriptions
</commit_message>
<xml_diff>
--- a/db_structure.xlsx
+++ b/db_structure.xlsx
@@ -11,13 +11,14 @@
     <sheet name="sqlite_sequence" sheetId="2" r:id="rId2"/>
     <sheet name="GOOGLE_SOLAR" sheetId="3" r:id="rId3"/>
     <sheet name="CEJST" sheetId="4" r:id="rId4"/>
+    <sheet name="PROPERTY_CODES" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="44">
   <si>
     <t>cid</t>
   </si>
@@ -140,6 +141,15 @@
   </si>
   <si>
     <t>identified_as_disadvantaged</t>
+  </si>
+  <si>
+    <t>property_code_id</t>
+  </si>
+  <si>
+    <t>property_code</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -1172,4 +1182,125 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>